<commit_message>
Fix an import issue with Excel files.
</commit_message>
<xml_diff>
--- a/VM-Core/src/test/java/com/validation/manager/core/tool/table/extractor/Tables.xlsx
+++ b/VM-Core/src/test/java/com/validation/manager/core/tool/table/extractor/Tables.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="8">
   <si>
     <t>N/A</t>
   </si>
@@ -24,10 +24,22 @@
     <t>SR0001</t>
   </si>
   <si>
-    <t>step</t>
-  </si>
-  <si>
-    <t>result</t>
+    <t>step 1</t>
+  </si>
+  <si>
+    <t>step 2</t>
+  </si>
+  <si>
+    <t>step 3</t>
+  </si>
+  <si>
+    <t>result 1</t>
+  </si>
+  <si>
+    <t>result 2</t>
+  </si>
+  <si>
+    <t>result 3</t>
   </si>
 </sst>
 </file>
@@ -362,7 +374,7 @@
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:C3"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -375,7 +387,7 @@
         <v>2</v>
       </c>
       <c r="C1" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:3">
@@ -383,10 +395,10 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C2" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -394,10 +406,10 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C3" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>